<commit_message>
dailylog and changed scheduele
</commit_message>
<xml_diff>
--- a/notes/climate_chamber/schedule/warm_fall/WarmF11sept.xlsx
+++ b/notes/climate_chamber/schedule/warm_fall/WarmF11sept.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/notes/climate_chamber/schedule/warm_fall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACAA6C6-0E94-2E4D-8192-3FA2CABA6C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33CA976-915E-B94E-91FB-6FDB6ED03CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37820" yWindow="-1980" windowWidth="27240" windowHeight="16260" xr2:uid="{4D476646-5361-4E43-ACF1-036E5CDB58BE}"/>
+    <workbookView xWindow="460" yWindow="740" windowWidth="27240" windowHeight="16260" xr2:uid="{4D476646-5361-4E43-ACF1-036E5CDB58BE}"/>
   </bookViews>
   <sheets>
     <sheet name="WarmF4sept" sheetId="1" r:id="rId1"/>
@@ -941,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF5A211E-EA4B-BE47-BD76-EEBE244813BA}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="139" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1395,7 +1395,7 @@
         <v>0.375</v>
       </c>
       <c r="C11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1747,7 +1747,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C19">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D19">
         <v>0</v>

</xml_diff>